<commit_message>
Mise à jour avancement
</commit_message>
<xml_diff>
--- a/KiCad/Avancée RISM 2011.xlsx
+++ b/KiCad/Avancée RISM 2011.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="435" windowWidth="18210" windowHeight="7605"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="32">
   <si>
     <t>Avancée électronique</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Priorité</t>
   </si>
   <si>
-    <t>Commencé</t>
-  </si>
-  <si>
     <t>Responsabilité</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>problème</t>
+  </si>
+  <si>
+    <t>presque fini</t>
   </si>
 </sst>
 </file>
@@ -161,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -206,21 +206,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -279,19 +264,6 @@
       </right>
       <top/>
       <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -567,117 +539,108 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -981,7 +944,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1020,26 +983,28 @@
       <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="16" t="s">
-        <v>22</v>
+      <c r="K3" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-      <c r="J4" s="13">
+      <c r="D4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="J4" s="11">
         <v>6</v>
       </c>
-      <c r="K4" s="20" t="s">
-        <v>26</v>
+      <c r="K4" s="18" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
@@ -1061,29 +1026,31 @@
       <c r="H5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="12">
         <v>2</v>
       </c>
-      <c r="K5" s="18" t="s">
-        <v>26</v>
+      <c r="K5" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="24"/>
-      <c r="J6" s="14">
+      <c r="D6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="21"/>
+      <c r="J6" s="12">
         <v>5</v>
       </c>
-      <c r="K6" s="18" t="s">
-        <v>26</v>
+      <c r="K6" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
@@ -1102,14 +1069,14 @@
       <c r="G7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="14">
+      <c r="H7" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="12">
         <v>3</v>
       </c>
-      <c r="K7" s="18" t="s">
-        <v>27</v>
+      <c r="K7" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
@@ -1131,8 +1098,8 @@
       <c r="H8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="17"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="C9" s="2" t="s">
@@ -1153,8 +1120,8 @@
       <c r="H9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="17"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="C10" s="2" t="s">
@@ -1172,50 +1139,50 @@
       <c r="G10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" s="14">
+      <c r="H10" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="12">
         <v>1</v>
       </c>
-      <c r="K10" s="18" t="s">
-        <v>23</v>
+      <c r="K10" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="24"/>
-      <c r="J11" s="14">
+      <c r="D11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="21"/>
+      <c r="J11" s="12">
         <v>5</v>
       </c>
-      <c r="K11" s="18" t="s">
-        <v>24</v>
+      <c r="K11" s="16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="24"/>
-      <c r="J12" s="14">
+      <c r="D12" s="22"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="21"/>
+      <c r="J12" s="12">
         <v>7</v>
       </c>
-      <c r="K12" s="18" t="s">
-        <v>28</v>
+      <c r="K12" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
@@ -1231,13 +1198,15 @@
       <c r="F13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="24"/>
-      <c r="J13" s="14">
+      <c r="G13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="J13" s="12">
         <v>4</v>
       </c>
-      <c r="K13" s="18" t="s">
-        <v>27</v>
+      <c r="K13" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
@@ -1259,9 +1228,9 @@
       <c r="H14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="37" t="s">
-        <v>25</v>
+      <c r="J14" s="13"/>
+      <c r="K14" s="35" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
@@ -1283,8 +1252,8 @@
       <c r="H15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="38"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="36"/>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="C16" s="2" t="s">
@@ -1305,8 +1274,8 @@
       <c r="H16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="36"/>
     </row>
     <row r="17" spans="3:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="C17" s="2" t="s">
@@ -1327,8 +1296,8 @@
       <c r="H17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="36"/>
     </row>
     <row r="18" spans="3:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="C18" s="2" t="s">
@@ -1343,76 +1312,76 @@
       <c r="F18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="24"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="38"/>
+      <c r="G18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="36"/>
     </row>
     <row r="19" spans="3:11" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="31"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="38"/>
+      <c r="D19" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="36"/>
     </row>
     <row r="20" spans="3:11" ht="15.75" thickBot="1">
-      <c r="C20" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="38"/>
+      <c r="C20" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" s="36"/>
     </row>
     <row r="21" spans="3:11" ht="15.75" thickBot="1">
       <c r="C21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="39"/>
+        <v>29</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="17"/>
+      <c r="K21" s="37"/>
     </row>
     <row r="22" spans="3:11" ht="15.75" thickTop="1"/>
   </sheetData>

</xml_diff>